<commit_message>
not making use of this as I would like. Will make a renewed effort.
</commit_message>
<xml_diff>
--- a/notebook.xlsx
+++ b/notebook.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -37,6 +37,26 @@
   </si>
   <si>
     <t>working on claim that for every pair of functions f and g, max(f, g) = theta(f(n) + g(n)). For n, we have some max between f(n) and g(n). Certainly max(f(n), g(n)) &lt;= f(n) + g(n).</t>
+  </si>
+  <si>
+    <t>Notebook</t>
+  </si>
+  <si>
+    <t>Started this notebook. Created git repo and started syncing. One issue with excel is that it locks and must close to commit to repo.</t>
+  </si>
+  <si>
+    <t>DOL - Venture</t>
+  </si>
+  <si>
+    <t>Steps to locate sproc. To be continued.</t>
+  </si>
+  <si>
+    <t>Continued from last time.  Assumption made is that f(n) and g(n) are always positive numbers. That condition should find big O. Then we need big omega… between those two should be theta. So, for omega: 2(max(f(n), g(n))) &gt;= f(n) + g(n) --&gt; max(f(n), g(n)) &gt;=  0.5(f(n) + g(n)). Thus: 1/2(f(n) + g(n)) &lt;= max(f(n), g(n)) &lt;= f(n) + g(n), for every n.  So, to satisfy theta, our constant C must be between 1 and 1/2... and n sub 0 is 1.
+New vid: O(n log n) Algorithm for Counting Inversions.
+1. Divide prob into smaller subproblems
+2. Subproblems solved via recursion
+3. Combine subproblem solutions into one solution for the real problem.
+Problem: Input of array A containing numbers in some arbitrary order. Output is the number of inversions (number of pairs where indices i and j is such that i &lt; j and A[i] &gt; A[j]. (sorted order has 0 inversions, but any other array with have some non-zero number</t>
   </si>
 </sst>
 </file>
@@ -44,8 +64,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="167" formatCode="hh:mm"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="165" formatCode="hh:mm"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -78,10 +98,10 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -384,11 +404,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -432,6 +452,59 @@
         <v>6</v>
       </c>
     </row>
+    <row r="3" spans="1:5" ht="30">
+      <c r="A3" s="1">
+        <v>41759</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.44861111111111113</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1">
+        <v>41759</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.45208333333333334</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="195">
+      <c r="A5" s="1">
+        <v>41759</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.45555555555555555</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1">
+        <v>41759</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.49444444444444446</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>